<commit_message>
Minor updates for readability
</commit_message>
<xml_diff>
--- a/DSN_Complex_Details.xlsx
+++ b/DSN_Complex_Details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudia/Dropbox (Indigo Wire Networks)/scripts/python/2020/fuzzy_wuzzy_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92826854-FFD5-4040-9797-54DC6B7B2D7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A40D11-44F1-5943-9A70-88BC67C73A5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3340" yWindow="11580" windowWidth="27640" windowHeight="16940" xr2:uid="{D7F215F4-763C-DF42-ADBA-2E1517B35C31}"/>
+    <workbookView xWindow="1700" yWindow="7460" windowWidth="43320" windowHeight="13720" xr2:uid="{D7F215F4-763C-DF42-ADBA-2E1517B35C31}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -167,7 +167,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="-0.249977111117893"/>
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -506,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB96C52D-E941-2D41-A6C0-B1B6CE0032C6}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>